<commit_message>
(C)    update tabs->spaces & publish test report        - update doc/style to 'v2'        - update idf demos
</commit_message>
<xml_diff>
--- a/doc/esp_proj/idf_demos/esp_idf_sel.xlsx
+++ b/doc/esp_proj/idf_demos/esp_idf_sel.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\MyWorkspaces\Espressif\esp32_proj\doc\esp_proj\idf_demos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2A18978-3B50-4306-B965-F5A1D8F968E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{272EDC10-2A7D-4A55-AD00-79C3BCA73607}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10695" yWindow="0" windowWidth="11010" windowHeight="13605" xr2:uid="{5FDA0259-A11B-4D0D-B086-92FD1D2DA28C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13740" xr2:uid="{5FDA0259-A11B-4D0D-B086-92FD1D2DA28C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="58">
   <si>
     <t>basic</t>
   </si>
@@ -186,6 +186,30 @@
   </si>
   <si>
     <t xml:space="preserve">Sync. I/O multiplexing </t>
+  </si>
+  <si>
+    <t>esp32_pwm</t>
+  </si>
+  <si>
+    <t>esp32_timer</t>
+  </si>
+  <si>
+    <t>gptimer_capture_hc_sr04</t>
+  </si>
+  <si>
+    <t>wiegand_interface</t>
+  </si>
+  <si>
+    <t>esp32_uart</t>
+  </si>
+  <si>
+    <t>uart_echo</t>
+  </si>
+  <si>
+    <t>uart_repl</t>
+  </si>
+  <si>
+    <t>uart_select</t>
   </si>
 </sst>
 </file>
@@ -236,7 +260,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="17">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -468,11 +492,61 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -524,6 +598,26 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -858,20 +952,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{257C0948-5064-4583-A3FD-082E9D1EFD4D}">
-  <dimension ref="A1:J36"/>
+  <dimension ref="A1:M54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="J41" sqref="J41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="26" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20.7109375" style="20" bestFit="1" customWidth="1"/>
-    <col min="3" max="10" width="13.7109375" customWidth="1"/>
+    <col min="3" max="13" width="13.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="11" t="s">
         <v>35</v>
       </c>
@@ -881,29 +975,38 @@
       <c r="C1" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="E1" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="F1" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="F1" s="12" t="s">
+      <c r="G1" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="G1" s="12" t="s">
+      <c r="H1" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="I1" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="J1" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="H1" s="12" t="s">
+      <c r="K1" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="I1" s="12" t="s">
+      <c r="L1" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="J1" s="13" t="s">
+      <c r="M1" s="13" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
         <v>0</v>
       </c>
@@ -911,15 +1014,18 @@
         <v>45</v>
       </c>
       <c r="C2" s="21"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="9"/>
       <c r="F2" s="8"/>
       <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8"/>
-      <c r="J2" s="10"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H2" s="28"/>
+      <c r="I2" s="28"/>
+      <c r="J2" s="8"/>
+      <c r="K2" s="8"/>
+      <c r="L2" s="8"/>
+      <c r="M2" s="10"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
         <v>1</v>
       </c>
@@ -927,13 +1033,16 @@
       <c r="C3" s="18"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="3"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F3" s="1"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="29"/>
+      <c r="I3" s="29"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+      <c r="M3" s="3"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
         <v>2</v>
       </c>
@@ -943,11 +1052,14 @@
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="3"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H4" s="29"/>
+      <c r="I4" s="29"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="3"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
         <v>3</v>
       </c>
@@ -957,53 +1069,65 @@
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="3"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H5" s="29"/>
+      <c r="I5" s="29"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="3"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="15" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="23"/>
       <c r="C6" s="22"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="2"/>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
-      <c r="J6" s="3"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H6" s="29"/>
+      <c r="I6" s="29"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+      <c r="M6" s="3"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="15" t="s">
         <v>5</v>
       </c>
       <c r="B7" s="23"/>
       <c r="C7" s="18"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="2"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
-      <c r="J7" s="3"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H7" s="29"/>
+      <c r="I7" s="29"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+      <c r="L7" s="1"/>
+      <c r="M7" s="3"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="15" t="s">
         <v>6</v>
       </c>
       <c r="B8" s="23"/>
       <c r="C8" s="18"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="2"/>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
-      <c r="J8" s="3"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H8" s="29"/>
+      <c r="I8" s="29"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
+      <c r="L8" s="1"/>
+      <c r="M8" s="3"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="s">
         <v>7</v>
       </c>
@@ -1012,40 +1136,49 @@
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
-      <c r="J9" s="3"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G9" s="1"/>
+      <c r="H9" s="29"/>
+      <c r="I9" s="29"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="1"/>
+      <c r="L9" s="1"/>
+      <c r="M9" s="3"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="15" t="s">
         <v>8</v>
       </c>
       <c r="B10" s="23"/>
       <c r="C10" s="18"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="2"/>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
-      <c r="J10" s="3"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H10" s="29"/>
+      <c r="I10" s="29"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="1"/>
+      <c r="L10" s="1"/>
+      <c r="M10" s="3"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="15" t="s">
         <v>9</v>
       </c>
       <c r="B11" s="23"/>
       <c r="C11" s="18"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="2"/>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
-      <c r="J11" s="3"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H11" s="29"/>
+      <c r="I11" s="29"/>
+      <c r="J11" s="1"/>
+      <c r="K11" s="1"/>
+      <c r="L11" s="1"/>
+      <c r="M11" s="3"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="15" t="s">
         <v>10</v>
       </c>
@@ -1055,11 +1188,14 @@
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
-      <c r="H12" s="2"/>
-      <c r="I12" s="1"/>
-      <c r="J12" s="3"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H12" s="29"/>
+      <c r="I12" s="29"/>
+      <c r="J12" s="1"/>
+      <c r="K12" s="2"/>
+      <c r="L12" s="1"/>
+      <c r="M12" s="3"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="15" t="s">
         <v>11</v>
       </c>
@@ -1069,25 +1205,31 @@
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
-      <c r="H13" s="2"/>
-      <c r="I13" s="1"/>
-      <c r="J13" s="3"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H13" s="29"/>
+      <c r="I13" s="29"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="2"/>
+      <c r="L13" s="1"/>
+      <c r="M13" s="3"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="15" t="s">
         <v>12</v>
       </c>
       <c r="B14" s="23"/>
       <c r="C14" s="18"/>
       <c r="D14" s="1"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="2"/>
       <c r="G14" s="1"/>
-      <c r="H14" s="1"/>
-      <c r="I14" s="1"/>
-      <c r="J14" s="3"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H14" s="29"/>
+      <c r="I14" s="29"/>
+      <c r="J14" s="1"/>
+      <c r="K14" s="1"/>
+      <c r="L14" s="1"/>
+      <c r="M14" s="3"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="15" t="s">
         <v>13</v>
       </c>
@@ -1095,87 +1237,105 @@
         <v>46</v>
       </c>
       <c r="C15" s="18"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="2"/>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
-      <c r="H15" s="1"/>
-      <c r="I15" s="1"/>
-      <c r="J15" s="3"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H15" s="29"/>
+      <c r="I15" s="29"/>
+      <c r="J15" s="1"/>
+      <c r="K15" s="1"/>
+      <c r="L15" s="1"/>
+      <c r="M15" s="3"/>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="15" t="s">
         <v>14</v>
       </c>
       <c r="B16" s="23"/>
       <c r="C16" s="18"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="2"/>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
-      <c r="H16" s="1"/>
-      <c r="I16" s="1"/>
-      <c r="J16" s="3"/>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H16" s="29"/>
+      <c r="I16" s="2"/>
+      <c r="J16" s="1"/>
+      <c r="K16" s="1"/>
+      <c r="L16" s="1"/>
+      <c r="M16" s="3"/>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="15" t="s">
-        <v>15</v>
+        <v>52</v>
       </c>
       <c r="B17" s="23"/>
-      <c r="C17" s="22"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="1"/>
+      <c r="C17" s="18"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="2"/>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
-      <c r="H17" s="1"/>
-      <c r="I17" s="1"/>
-      <c r="J17" s="3"/>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H17" s="29"/>
+      <c r="I17" s="2"/>
+      <c r="J17" s="1"/>
+      <c r="K17" s="1"/>
+      <c r="L17" s="1"/>
+      <c r="M17" s="3"/>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B18" s="23"/>
+      <c r="C18" s="22"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="29"/>
+      <c r="I18" s="29"/>
+      <c r="J18" s="1"/>
+      <c r="K18" s="1"/>
+      <c r="L18" s="1"/>
+      <c r="M18" s="3"/>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A19" s="15" t="s">
         <v>16</v>
-      </c>
-      <c r="B18" s="23"/>
-      <c r="C18" s="18"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
-      <c r="G18" s="2"/>
-      <c r="H18" s="1"/>
-      <c r="I18" s="1"/>
-      <c r="J18" s="3"/>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="15" t="s">
-        <v>17</v>
       </c>
       <c r="B19" s="23"/>
       <c r="C19" s="18"/>
-      <c r="D19" s="2"/>
+      <c r="D19" s="1"/>
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
-      <c r="H19" s="1"/>
-      <c r="I19" s="1"/>
-      <c r="J19" s="3"/>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H19" s="29"/>
+      <c r="I19" s="29"/>
+      <c r="J19" s="2"/>
+      <c r="K19" s="1"/>
+      <c r="L19" s="1"/>
+      <c r="M19" s="3"/>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="15" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B20" s="23"/>
       <c r="C20" s="18"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="2"/>
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
-      <c r="H20" s="1"/>
-      <c r="I20" s="1"/>
-      <c r="J20" s="3"/>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H20" s="29"/>
+      <c r="I20" s="29"/>
+      <c r="J20" s="1"/>
+      <c r="K20" s="1"/>
+      <c r="L20" s="1"/>
+      <c r="M20" s="3"/>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="15" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B21" s="23"/>
       <c r="C21" s="18"/>
@@ -1183,27 +1343,33 @@
       <c r="E21" s="2"/>
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
-      <c r="H21" s="1"/>
-      <c r="I21" s="1"/>
-      <c r="J21" s="3"/>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H21" s="29"/>
+      <c r="I21" s="29"/>
+      <c r="J21" s="1"/>
+      <c r="K21" s="1"/>
+      <c r="L21" s="1"/>
+      <c r="M21" s="3"/>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B22" s="23"/>
       <c r="C22" s="18"/>
-      <c r="D22" s="1"/>
+      <c r="D22" s="2"/>
       <c r="E22" s="1"/>
       <c r="F22" s="2"/>
       <c r="G22" s="1"/>
-      <c r="H22" s="1"/>
-      <c r="I22" s="1"/>
-      <c r="J22" s="3"/>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H22" s="29"/>
+      <c r="I22" s="29"/>
+      <c r="J22" s="1"/>
+      <c r="K22" s="1"/>
+      <c r="L22" s="1"/>
+      <c r="M22" s="3"/>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="15" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B23" s="23"/>
       <c r="C23" s="18"/>
@@ -1211,89 +1377,107 @@
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
       <c r="G23" s="2"/>
-      <c r="H23" s="1"/>
-      <c r="I23" s="1"/>
-      <c r="J23" s="3"/>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H23" s="29"/>
+      <c r="I23" s="29"/>
+      <c r="J23" s="1"/>
+      <c r="K23" s="1"/>
+      <c r="L23" s="1"/>
+      <c r="M23" s="3"/>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B24" s="23"/>
       <c r="C24" s="18"/>
       <c r="D24" s="1"/>
-      <c r="E24" s="2"/>
+      <c r="E24" s="1"/>
       <c r="F24" s="1"/>
       <c r="G24" s="1"/>
-      <c r="H24" s="1"/>
-      <c r="I24" s="1"/>
-      <c r="J24" s="3"/>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H24" s="29"/>
+      <c r="I24" s="29"/>
+      <c r="J24" s="2"/>
+      <c r="K24" s="1"/>
+      <c r="L24" s="1"/>
+      <c r="M24" s="3"/>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="B25" s="23"/>
+      <c r="C25" s="18"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="2"/>
+      <c r="G25" s="1"/>
+      <c r="H25" s="29"/>
+      <c r="I25" s="29"/>
+      <c r="J25" s="1"/>
+      <c r="K25" s="1"/>
+      <c r="L25" s="1"/>
+      <c r="M25" s="3"/>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A26" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="B25" s="26" t="s">
+      <c r="B26" s="26" t="s">
         <v>49</v>
       </c>
-      <c r="C25" s="18" t="s">
+      <c r="C26" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="D25" s="2"/>
-      <c r="E25" s="1"/>
-      <c r="F25" s="1"/>
-      <c r="G25" s="1"/>
-      <c r="H25" s="1"/>
-      <c r="I25" s="1"/>
-      <c r="J25" s="3"/>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26" s="15" t="s">
+      <c r="D26" s="1"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1"/>
+      <c r="H26" s="29"/>
+      <c r="I26" s="29"/>
+      <c r="J26" s="1"/>
+      <c r="K26" s="1"/>
+      <c r="L26" s="1"/>
+      <c r="M26" s="3"/>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A27" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="B26" s="23" t="s">
+      <c r="B27" s="23" t="s">
         <v>47</v>
       </c>
-      <c r="C26" s="18"/>
-      <c r="D26" s="1"/>
-      <c r="E26" s="1"/>
-      <c r="F26" s="1"/>
-      <c r="G26" s="2"/>
-      <c r="H26" s="1"/>
-      <c r="I26" s="1"/>
-      <c r="J26" s="3"/>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="B27" s="23"/>
       <c r="C27" s="18"/>
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
-      <c r="G27" s="2"/>
-      <c r="H27" s="1"/>
-      <c r="I27" s="1"/>
-      <c r="J27" s="3"/>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G27" s="1"/>
+      <c r="H27" s="29"/>
+      <c r="I27" s="29"/>
+      <c r="J27" s="2"/>
+      <c r="K27" s="1"/>
+      <c r="L27" s="1"/>
+      <c r="M27" s="3"/>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B28" s="23"/>
       <c r="C28" s="18"/>
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
       <c r="F28" s="1"/>
-      <c r="G28" s="2"/>
-      <c r="H28" s="1"/>
-      <c r="I28" s="1"/>
-      <c r="J28" s="3"/>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G28" s="1"/>
+      <c r="H28" s="29"/>
+      <c r="I28" s="29"/>
+      <c r="J28" s="2"/>
+      <c r="K28" s="1"/>
+      <c r="L28" s="1"/>
+      <c r="M28" s="3"/>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B29" s="23"/>
       <c r="C29" s="18"/>
@@ -1301,107 +1485,255 @@
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
       <c r="G29" s="1"/>
-      <c r="H29" s="1"/>
-      <c r="I29" s="1"/>
-      <c r="J29" s="4"/>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H29" s="29"/>
+      <c r="I29" s="29"/>
+      <c r="J29" s="2"/>
+      <c r="K29" s="1"/>
+      <c r="L29" s="1"/>
+      <c r="M29" s="3"/>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="15" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B30" s="23"/>
       <c r="C30" s="18"/>
       <c r="D30" s="1"/>
       <c r="E30" s="1"/>
       <c r="F30" s="1"/>
-      <c r="G30" s="2"/>
-      <c r="H30" s="1"/>
-      <c r="I30" s="1"/>
-      <c r="J30" s="3"/>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G30" s="1"/>
+      <c r="H30" s="29"/>
+      <c r="I30" s="29"/>
+      <c r="J30" s="1"/>
+      <c r="K30" s="1"/>
+      <c r="L30" s="1"/>
+      <c r="M30" s="4"/>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" s="15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B31" s="23"/>
       <c r="C31" s="18"/>
       <c r="D31" s="1"/>
       <c r="E31" s="1"/>
       <c r="F31" s="1"/>
-      <c r="G31" s="2"/>
-      <c r="H31" s="1"/>
-      <c r="I31" s="1"/>
-      <c r="J31" s="3"/>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G31" s="1"/>
+      <c r="H31" s="29"/>
+      <c r="I31" s="29"/>
+      <c r="J31" s="2"/>
+      <c r="K31" s="1"/>
+      <c r="L31" s="1"/>
+      <c r="M31" s="3"/>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" s="15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B32" s="23"/>
       <c r="C32" s="18"/>
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>
       <c r="F32" s="1"/>
-      <c r="G32" s="2"/>
-      <c r="H32" s="1"/>
-      <c r="I32" s="1"/>
-      <c r="J32" s="3"/>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G32" s="1"/>
+      <c r="H32" s="29"/>
+      <c r="I32" s="29"/>
+      <c r="J32" s="2"/>
+      <c r="K32" s="1"/>
+      <c r="L32" s="1"/>
+      <c r="M32" s="3"/>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="B33" s="39"/>
+      <c r="C33" s="27"/>
+      <c r="D33" s="29"/>
+      <c r="E33" s="29"/>
+      <c r="F33" s="29"/>
+      <c r="G33" s="29"/>
+      <c r="H33" s="2"/>
+      <c r="I33" s="29"/>
+      <c r="J33" s="29"/>
+      <c r="K33" s="29"/>
+      <c r="L33" s="29"/>
+      <c r="M33" s="40"/>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A34" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="B34" s="39"/>
+      <c r="C34" s="27"/>
+      <c r="D34" s="29"/>
+      <c r="E34" s="29"/>
+      <c r="F34" s="29"/>
+      <c r="G34" s="29"/>
+      <c r="H34" s="2"/>
+      <c r="I34" s="29"/>
+      <c r="J34" s="29"/>
+      <c r="K34" s="29"/>
+      <c r="L34" s="29"/>
+      <c r="M34" s="40"/>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A35" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="B35" s="39"/>
+      <c r="C35" s="27"/>
+      <c r="D35" s="29"/>
+      <c r="E35" s="29"/>
+      <c r="F35" s="29"/>
+      <c r="G35" s="29"/>
+      <c r="H35" s="2"/>
+      <c r="I35" s="29"/>
+      <c r="J35" s="29"/>
+      <c r="K35" s="29"/>
+      <c r="L35" s="29"/>
+      <c r="M35" s="40"/>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A36" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="B36" s="23"/>
+      <c r="C36" s="18"/>
+      <c r="D36" s="1"/>
+      <c r="E36" s="1"/>
+      <c r="F36" s="1"/>
+      <c r="G36" s="1"/>
+      <c r="H36" s="29"/>
+      <c r="I36" s="29"/>
+      <c r="J36" s="2"/>
+      <c r="K36" s="1"/>
+      <c r="L36" s="1"/>
+      <c r="M36" s="3"/>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A37" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="B33" s="23"/>
-      <c r="C33" s="18"/>
-      <c r="D33" s="1"/>
-      <c r="E33" s="1"/>
-      <c r="F33" s="1"/>
-      <c r="G33" s="2"/>
-      <c r="H33" s="1"/>
-      <c r="I33" s="1"/>
-      <c r="J33" s="3"/>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A34" s="15" t="s">
+      <c r="B37" s="23"/>
+      <c r="C37" s="18"/>
+      <c r="D37" s="1"/>
+      <c r="E37" s="1"/>
+      <c r="F37" s="1"/>
+      <c r="G37" s="1"/>
+      <c r="H37" s="29"/>
+      <c r="I37" s="29"/>
+      <c r="J37" s="2"/>
+      <c r="K37" s="1"/>
+      <c r="L37" s="1"/>
+      <c r="M37" s="3"/>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A38" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="B34" s="23"/>
-      <c r="C34" s="18"/>
-      <c r="D34" s="2"/>
-      <c r="E34" s="1"/>
-      <c r="F34" s="1"/>
-      <c r="G34" s="1"/>
-      <c r="H34" s="1"/>
-      <c r="I34" s="1"/>
-      <c r="J34" s="3"/>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A35" s="15" t="s">
+      <c r="B38" s="23"/>
+      <c r="C38" s="18"/>
+      <c r="D38" s="1"/>
+      <c r="E38" s="2"/>
+      <c r="F38" s="1"/>
+      <c r="G38" s="1"/>
+      <c r="H38" s="29"/>
+      <c r="I38" s="29"/>
+      <c r="J38" s="1"/>
+      <c r="K38" s="1"/>
+      <c r="L38" s="1"/>
+      <c r="M38" s="3"/>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A39" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="B35" s="23"/>
-      <c r="C35" s="18"/>
-      <c r="D35" s="2"/>
-      <c r="E35" s="1"/>
-      <c r="F35" s="1"/>
-      <c r="G35" s="1"/>
-      <c r="H35" s="1"/>
-      <c r="I35" s="1"/>
-      <c r="J35" s="3"/>
-    </row>
-    <row r="36" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="16" t="s">
+      <c r="B39" s="23"/>
+      <c r="C39" s="18"/>
+      <c r="D39" s="1"/>
+      <c r="E39" s="2"/>
+      <c r="F39" s="1"/>
+      <c r="G39" s="1"/>
+      <c r="H39" s="29"/>
+      <c r="I39" s="29"/>
+      <c r="J39" s="1"/>
+      <c r="K39" s="1"/>
+      <c r="L39" s="1"/>
+      <c r="M39" s="3"/>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A40" s="32" t="s">
+        <v>53</v>
+      </c>
+      <c r="B40" s="33"/>
+      <c r="C40" s="34"/>
+      <c r="D40" s="35"/>
+      <c r="E40" s="1"/>
+      <c r="F40" s="35"/>
+      <c r="G40" s="35"/>
+      <c r="H40" s="37"/>
+      <c r="I40" s="36"/>
+      <c r="J40" s="35"/>
+      <c r="K40" s="35"/>
+      <c r="L40" s="35"/>
+      <c r="M40" s="38"/>
+    </row>
+    <row r="41" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="B36" s="24"/>
-      <c r="C36" s="19"/>
-      <c r="D36" s="5"/>
-      <c r="E36" s="5"/>
-      <c r="F36" s="5"/>
-      <c r="G36" s="6"/>
-      <c r="H36" s="5"/>
-      <c r="I36" s="5"/>
-      <c r="J36" s="7"/>
+      <c r="B41" s="24"/>
+      <c r="C41" s="19"/>
+      <c r="D41" s="5"/>
+      <c r="E41" s="5"/>
+      <c r="F41" s="5"/>
+      <c r="G41" s="5"/>
+      <c r="H41" s="30"/>
+      <c r="I41" s="30"/>
+      <c r="J41" s="6"/>
+      <c r="K41" s="5"/>
+      <c r="L41" s="5"/>
+      <c r="M41" s="7"/>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="I42" s="31"/>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="I43" s="31"/>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="I44" s="31"/>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="I45" s="31"/>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="I46" s="31"/>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="I47" s="31"/>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="I48" s="31"/>
+    </row>
+    <row r="49" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I49" s="31"/>
+    </row>
+    <row r="50" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I50" s="31"/>
+    </row>
+    <row r="51" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I51" s="31"/>
+    </row>
+    <row r="52" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I52" s="31"/>
+    </row>
+    <row r="53" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I53" s="31"/>
+    </row>
+    <row r="54" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I54" s="31"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>